<commit_message>
TL: S51003, S51004, S51006, S51009 ReTL: P06110, P32110, S50000, S50001, S50003, S50004
</commit_message>
<xml_diff>
--- a/tl/P06110.MES.BIN.xlsx
+++ b/tl/P06110.MES.BIN.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F627CE93-2782-45B2-9DA6-99EFC8401A4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6739BA4-CC09-476D-802D-7D9992F42D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2985" yWindow="16245" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5460" yWindow="16200" windowWidth="49560" windowHeight="15225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="P06110.MES.BIN" sheetId="1" r:id="rId1"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="81">
   <si>
     <t>Status</t>
   </si>
@@ -144,6 +144,9 @@
   </si>
   <si>
     <t>27</t>
+  </si>
+  <si>
+    <t>Perhaps Yuki has a fairly good hobby.</t>
   </si>
   <si>
     <t>Yuki has pretty good taste.</t>
@@ -1151,13 +1154,13 @@
         <v>9</v>
       </c>
       <c r="F15" s="4" t="s">
-        <v>9</v>
+        <v>43</v>
       </c>
       <c r="G15" s="5" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="I15" s="5" t="s">
         <v>9</v>
@@ -1171,7 +1174,7 @@
         <v>9</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>14</v>
@@ -1186,7 +1189,7 @@
         <v>9</v>
       </c>
       <c r="G16" s="3" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="H16" s="3" t="s">
         <v>9</v>
@@ -1203,7 +1206,7 @@
         <v>9</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C17" s="4" t="s">
         <v>10</v>
@@ -1218,7 +1221,7 @@
         <v>9</v>
       </c>
       <c r="G17" s="5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="H17" s="5" t="s">
         <v>9</v>
@@ -1235,7 +1238,7 @@
         <v>9</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>14</v>
@@ -1250,7 +1253,7 @@
         <v>9</v>
       </c>
       <c r="G18" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="H18" s="3" t="s">
         <v>9</v>
@@ -1267,7 +1270,7 @@
         <v>9</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C19" s="4" t="s">
         <v>10</v>
@@ -1279,10 +1282,10 @@
         <v>9</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="G19" s="5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="H19" s="5" t="s">
         <v>9</v>
@@ -1299,7 +1302,7 @@
         <v>9</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>14</v>
@@ -1314,7 +1317,7 @@
         <v>9</v>
       </c>
       <c r="G20" s="3" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="H20" s="3" t="s">
         <v>9</v>
@@ -1331,7 +1334,7 @@
         <v>9</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>10</v>
@@ -1346,7 +1349,7 @@
         <v>9</v>
       </c>
       <c r="G21" s="5" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="H21" s="5" t="s">
         <v>9</v>
@@ -1363,7 +1366,7 @@
         <v>9</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C22" s="2" t="s">
         <v>14</v>
@@ -1378,7 +1381,7 @@
         <v>9</v>
       </c>
       <c r="G22" s="3" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="H22" s="3" t="s">
         <v>9</v>
@@ -1395,7 +1398,7 @@
         <v>9</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C23" s="4" t="s">
         <v>9</v>
@@ -1410,7 +1413,7 @@
         <v>9</v>
       </c>
       <c r="G23" s="5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="H23" s="5" t="s">
         <v>9</v>
@@ -1427,7 +1430,7 @@
         <v>9</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="C24" s="2" t="s">
         <v>10</v>
@@ -1442,7 +1445,7 @@
         <v>9</v>
       </c>
       <c r="G24" s="3" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="H24" s="3" t="s">
         <v>9</v>
@@ -1459,7 +1462,7 @@
         <v>9</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>14</v>
@@ -1474,7 +1477,7 @@
         <v>9</v>
       </c>
       <c r="G25" s="5" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="H25" s="5" t="s">
         <v>9</v>
@@ -1491,7 +1494,7 @@
         <v>9</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C26" s="2" t="s">
         <v>10</v>
@@ -1506,7 +1509,7 @@
         <v>9</v>
       </c>
       <c r="G26" s="3" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="H26" s="3" t="s">
         <v>9</v>
@@ -1523,7 +1526,7 @@
         <v>9</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="C27" s="4" t="s">
         <v>9</v>
@@ -1538,7 +1541,7 @@
         <v>9</v>
       </c>
       <c r="G27" s="5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="H27" s="5" t="s">
         <v>9</v>
@@ -1555,7 +1558,7 @@
         <v>9</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>14</v>
@@ -1567,13 +1570,13 @@
         <v>9</v>
       </c>
       <c r="F28" s="2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="G28" s="3" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="I28" s="3" t="s">
         <v>9</v>
@@ -1587,7 +1590,7 @@
         <v>9</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>10</v>
@@ -1602,7 +1605,7 @@
         <v>9</v>
       </c>
       <c r="G29" s="5" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="H29" s="5" t="s">
         <v>9</v>
@@ -1619,7 +1622,7 @@
         <v>9</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>9</v>
@@ -1634,7 +1637,7 @@
         <v>9</v>
       </c>
       <c r="G30" s="3" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
       <c r="H30" s="3" t="s">
         <v>9</v>
@@ -1651,7 +1654,7 @@
         <v>9</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="C31" s="4" t="s">
         <v>9</v>
@@ -1666,7 +1669,7 @@
         <v>9</v>
       </c>
       <c r="G31" s="5" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="H31" s="5" t="s">
         <v>9</v>

</xml_diff>